<commit_message>
Actualización de Caja Blanca y Caja Negra
Aquí actualizando la Documentación.
</commit_message>
<xml_diff>
--- a/BIBLIOTECA DE TRABAJO/Documentación/BACKLOG _V7.0.xlsx
+++ b/BIBLIOTECA DE TRABAJO/Documentación/BACKLOG _V7.0.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ESPE\Primer Semestre\Fund. Ing\NRC1951_G7_FUN_ING_SW\DOCUMENTACIÓN_G#7\1.ELICITACIÓN\1.6 BACKLOG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ESPE\Primer Semestre\Fund. Ing\NRC1951_G7_FUN_ING_SW\BIBLIOTECA DE TRABAJO\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -3008,7 +3008,9 @@
   </sheetPr>
   <dimension ref="A1:I997"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -3198,7 +3200,7 @@
       <c r="B10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -4323,7 +4325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>